<commit_message>
f/mmcdaniel-baroreceptors: Reduce autoregulation during drug admin
There is some odd behavior that can get introduced when combining drugs
(like fentanyl) with autoregulation.  Remove autoregulatory effect
during drug admin--leave needed physiology changes to drug modifiers.
To phase out this behavior, we would need to model exactly how
individual drugs interact with the cns.

Also add more validation updates.
</commit_message>
<xml_diff>
--- a/share/doc/validation/Scenarios/CombinedValidation.xlsx
+++ b/share/doc/validation/Scenarios/CombinedValidation.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjectPrograms\BioGears\core\share\doc\validation\Scenarios\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="228" windowWidth="14640" windowHeight="3420"/>
   </bookViews>
@@ -22,7 +27,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="5">Nathan!#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Summary!$B$1:$D$7</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -359,7 +364,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1081,6 +1086,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1128,7 +1136,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1163,7 +1171,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1378,7 +1386,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>